<commit_message>
add command line args for h,w,c
</commit_message>
<xml_diff>
--- a/outputs/torch/gnmt.xlsx
+++ b/outputs/torch/gnmt.xlsx
@@ -753,9 +753,7 @@
       </c>
       <c r="P4" s="8" t="n"/>
       <c r="Q4" s="8" t="n"/>
-      <c r="R4" s="8" t="n">
-        <v>2097152</v>
-      </c>
+      <c r="R4" s="8" t="n"/>
       <c r="S4" s="8" t="n"/>
       <c r="T4" s="8" t="n"/>
     </row>
@@ -797,9 +795,7 @@
       </c>
       <c r="P5" s="8" t="n"/>
       <c r="Q5" s="8" t="n"/>
-      <c r="R5" s="8" t="n">
-        <v>2097152</v>
-      </c>
+      <c r="R5" s="8" t="n"/>
       <c r="S5" s="8" t="n"/>
       <c r="T5" s="8" t="n"/>
     </row>
@@ -917,21 +913,13 @@
       <c r="O8" s="8" t="n">
         <v>16777216</v>
       </c>
-      <c r="P8" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="P8" s="8" t="n"/>
       <c r="Q8" s="8" t="n">
         <v>5120</v>
       </c>
-      <c r="R8" s="8" t="n">
-        <v>16777216</v>
-      </c>
-      <c r="S8" s="8" t="n">
-        <v>20480</v>
-      </c>
-      <c r="T8" s="8" t="n">
-        <v>5120</v>
-      </c>
+      <c r="R8" s="8" t="n"/>
+      <c r="S8" s="8" t="n"/>
+      <c r="T8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="n">
@@ -1011,21 +999,13 @@
       <c r="O10" s="8" t="n">
         <v>12582912</v>
       </c>
-      <c r="P10" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="P10" s="8" t="n"/>
       <c r="Q10" s="8" t="n">
         <v>5120</v>
       </c>
-      <c r="R10" s="8" t="n">
-        <v>12582912</v>
-      </c>
-      <c r="S10" s="8" t="n">
-        <v>20480</v>
-      </c>
-      <c r="T10" s="8" t="n">
-        <v>5120</v>
-      </c>
+      <c r="R10" s="8" t="n"/>
+      <c r="S10" s="8" t="n"/>
+      <c r="T10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n">
@@ -1105,21 +1085,13 @@
       <c r="O12" s="8" t="n">
         <v>8388608</v>
       </c>
-      <c r="P12" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="P12" s="8" t="n"/>
       <c r="Q12" s="8" t="n">
         <v>5120</v>
       </c>
-      <c r="R12" s="8" t="n">
-        <v>8388608</v>
-      </c>
-      <c r="S12" s="8" t="n">
-        <v>20480</v>
-      </c>
-      <c r="T12" s="8" t="n">
-        <v>5120</v>
-      </c>
+      <c r="R12" s="8" t="n"/>
+      <c r="S12" s="8" t="n"/>
+      <c r="T12" s="8" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="7" t="n">
@@ -1203,9 +1175,7 @@
       </c>
       <c r="P14" s="8" t="n"/>
       <c r="Q14" s="8" t="n"/>
-      <c r="R14" s="8" t="n">
-        <v>2097152</v>
-      </c>
+      <c r="R14" s="8" t="n"/>
       <c r="S14" s="8" t="n"/>
       <c r="T14" s="8" t="n"/>
     </row>
@@ -1247,9 +1217,7 @@
       </c>
       <c r="P15" s="8" t="n"/>
       <c r="Q15" s="8" t="n"/>
-      <c r="R15" s="8" t="n">
-        <v>2097152</v>
-      </c>
+      <c r="R15" s="8" t="n"/>
       <c r="S15" s="8" t="n"/>
       <c r="T15" s="8" t="n"/>
     </row>
@@ -1375,21 +1343,13 @@
       <c r="O18" s="8" t="n">
         <v>8388608</v>
       </c>
-      <c r="P18" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="P18" s="8" t="n"/>
       <c r="Q18" s="8" t="n">
         <v>5120</v>
       </c>
-      <c r="R18" s="8" t="n">
-        <v>8388608</v>
-      </c>
-      <c r="S18" s="8" t="n">
-        <v>20480</v>
-      </c>
-      <c r="T18" s="8" t="n">
-        <v>5120</v>
-      </c>
+      <c r="R18" s="8" t="n"/>
+      <c r="S18" s="8" t="n"/>
+      <c r="T18" s="8" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="7" t="n">
@@ -1645,21 +1605,13 @@
       <c r="O24" s="8" t="n">
         <v>12582912</v>
       </c>
-      <c r="P24" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="P24" s="8" t="n"/>
       <c r="Q24" s="8" t="n">
         <v>5120</v>
       </c>
-      <c r="R24" s="8" t="n">
-        <v>12582912</v>
-      </c>
-      <c r="S24" s="8" t="n">
-        <v>20480</v>
-      </c>
-      <c r="T24" s="8" t="n">
-        <v>5120</v>
-      </c>
+      <c r="R24" s="8" t="n"/>
+      <c r="S24" s="8" t="n"/>
+      <c r="T24" s="8" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="7" t="n">
@@ -1739,21 +1691,13 @@
       <c r="O26" s="8" t="n">
         <v>12582912</v>
       </c>
-      <c r="P26" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="P26" s="8" t="n"/>
       <c r="Q26" s="8" t="n">
         <v>5120</v>
       </c>
-      <c r="R26" s="8" t="n">
-        <v>12582912</v>
-      </c>
-      <c r="S26" s="8" t="n">
-        <v>20480</v>
-      </c>
-      <c r="T26" s="8" t="n">
-        <v>5120</v>
-      </c>
+      <c r="R26" s="8" t="n"/>
+      <c r="S26" s="8" t="n"/>
+      <c r="T26" s="8" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="7" t="n">
@@ -1837,21 +1781,13 @@
       <c r="O28" s="8" t="n">
         <v>12582912</v>
       </c>
-      <c r="P28" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="P28" s="8" t="n"/>
       <c r="Q28" s="8" t="n">
         <v>5120</v>
       </c>
-      <c r="R28" s="8" t="n">
-        <v>12582912</v>
-      </c>
-      <c r="S28" s="8" t="n">
-        <v>20480</v>
-      </c>
-      <c r="T28" s="8" t="n">
-        <v>5120</v>
-      </c>
+      <c r="R28" s="8" t="n"/>
+      <c r="S28" s="8" t="n"/>
+      <c r="T28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="n">
@@ -1925,7 +1861,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R29">
     <cfRule type="cellIs" priority="4" operator="equal" dxfId="3" stopIfTrue="1">
-      <formula>16777216</formula>
+      <formula>2097152</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1994,7 +1930,7 @@
         </is>
       </c>
       <c r="B5" s="8" t="n">
-        <v>0.096468992</v>
+        <v>0.004194304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>